<commit_message>
POM - 1 : class login
</commit_message>
<xml_diff>
--- a/resources/data.xlsx
+++ b/resources/data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>username</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>mAnydes</t>
+  </si>
+  <si>
+    <t>mngr506568</t>
+  </si>
+  <si>
+    <t>sYdAjun</t>
   </si>
 </sst>
 </file>
@@ -487,10 +493,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>